<commit_message>
0.3.5 Result file usage examples
</commit_message>
<xml_diff>
--- a/research/star_systems/TOI-4504/TOI-4504.xlsx
+++ b/research/star_systems/TOI-4504/TOI-4504.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meine Ablage\Python\curvesim\research\star_systems\TOI-4504\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ulsc\OneDrive - AspIT - Ondrive\Uli\Python\curvesim\research\star_systems\TOI-4504\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEFBE35-60D9-4BF2-BBC9-D3C1C3E9BC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2397D3-2CAB-44E5-8F80-80AF96F857D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{6919DDE8-15F9-45FB-B5F7-4209377AF865}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6919DDE8-15F9-45FB-B5F7-4209377AF865}"/>
   </bookViews>
   <sheets>
     <sheet name="Planet c" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="97">
   <si>
     <r>
       <t xml:space="preserve">def </t>
@@ -2006,9 +2006,6 @@
     <t>depth</t>
   </si>
   <si>
-    <t>Manuell aus den Plots der mit lightcurve herunter geladenen .fits-Dateien geschaetzt:</t>
-  </si>
-  <si>
     <t>TT  [BJD]</t>
   </si>
   <si>
@@ -2016,14 +2013,66 @@
   </si>
   <si>
     <t>P</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>T10</t>
+  </si>
+  <si>
+    <t>T11</t>
+  </si>
+  <si>
+    <t>T0</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T19</t>
+  </si>
+  <si>
+    <t>T20</t>
+  </si>
+  <si>
+    <t>T21</t>
+  </si>
+  <si>
+    <t>Transit</t>
+  </si>
+  <si>
+    <t>Manuell aus lightkurve plots</t>
+  </si>
+  <si>
+    <t>y-Aufschlag</t>
+  </si>
+  <si>
+    <t>Amplitude</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequenz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -2155,7 +2204,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2168,11 +2217,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -2182,7 +2246,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2238,10 +2302,29 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Procent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2259,6 +2342,1126 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="da-DK"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Transits c'!$D$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>P</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="5"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Transits c'!$C$19:$C$39</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>2458483.2110000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2458565.0902</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2458647.3328</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2458730.3328</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2458813.3328</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2458896.3328</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2458979.3328</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2459062.3328</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2459148.4781999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2459231.1144000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2459313.2535000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2459396.2535000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2459479.2535000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2459562.2535000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2459645.2535000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2459728.2535000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2459811.2535000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2459894.2535000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2459977.2535000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2460059.6189000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2460142.6048000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Transits c'!$D$19:$D$39</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>81.802400000393391</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>81.879199999850243</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82.242599999997765</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>83.241199999582022</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>82.636200000531971</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>82.139099999796599</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>83.569600000046194</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>82.985900000203401</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DC2E-4F37-9EBC-BF518BCEC319}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Transits c'!$E$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="6"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Transits c'!$C$19:$C$39</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>2458483.2110000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2458565.0902</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2458647.3328</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2458730.3328</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2458813.3328</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2458896.3328</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2458979.3328</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2459062.3328</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2459148.4781999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2459231.1144000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2459313.2535000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2459396.2535000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2459479.2535000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2459562.2535000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2459645.2535000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2459728.2535000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2459811.2535000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2459894.2535000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2459977.2535000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2460059.6189000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2460142.6048000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Transits c'!$E$19:$E$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>81.702855122563122</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>81.7992822018347</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82.140213815813425</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82.638059258736973</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83.153035090454694</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>83.542719117801852</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>83.699339965118099</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>83.579582425754424</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>83.199195419955913</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>82.692855181495872</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>82.191215220517591</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>81.824765723684834</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>81.70037182924797</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>81.852436027908183</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>82.238903303990682</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>82.752891909545326</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>83.252252679589731</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>83.598881936883473</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>83.696915572864086</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>83.521567708892789</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>83.118777348149962</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DC2E-4F37-9EBC-BF518BCEC319}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1542051359"/>
+        <c:axId val="1526639535"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1542051359"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1526639535"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1526639535"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1542051359"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="da-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2882,8 +4085,93 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>678180</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagram 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF0D0403-7A8D-B4A2-B963-BE5F589C21FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>52792</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Billede 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86D8C2AF-1E1D-33D5-F18C-78E144CFA1D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5318760" y="0"/>
+          <a:ext cx="9273540" cy="2247352"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3201,37 +4489,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{297EEAD8-1435-4033-9511-E3E1B196AAA2}">
   <dimension ref="A1:O183"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A178" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>53</v>
       </c>
@@ -3251,22 +4539,22 @@
         <v>661.46475017111572</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>58</v>
       </c>
@@ -3277,18 +4565,18 @@
         <v>59</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>49</v>
       </c>
       <c r="O97" s="16"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>65</v>
       </c>
@@ -3312,12 +4600,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="152" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I152" s="18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>140000</v>
       </c>
@@ -3332,7 +4620,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166">
         <f>(2595000-2460000)/5</f>
         <v>27000</v>
@@ -3348,7 +4636,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="177" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="177" spans="14:15" x14ac:dyDescent="0.3">
       <c r="N177" s="20" t="s">
         <v>62</v>
       </c>
@@ -3356,7 +4644,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="178" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="178" spans="14:15" x14ac:dyDescent="0.3">
       <c r="N178" s="19">
         <v>7.5174886019559386</v>
       </c>
@@ -3364,7 +4652,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="179" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="179" spans="14:15" x14ac:dyDescent="0.3">
       <c r="N179" s="19">
         <v>20.046636271882502</v>
       </c>
@@ -3372,7 +4660,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="180" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="180" spans="14:15" x14ac:dyDescent="0.3">
       <c r="N180" s="19">
         <v>7.5174886019559386</v>
       </c>
@@ -3380,7 +4668,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="181" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="181" spans="14:15" x14ac:dyDescent="0.3">
       <c r="N181" s="19">
         <v>11.276232902933909</v>
       </c>
@@ -3388,7 +4676,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="182" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="182" spans="14:15" x14ac:dyDescent="0.3">
       <c r="N182" s="19">
         <v>16.287891970904536</v>
       </c>
@@ -3396,7 +4684,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="183" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="183" spans="14:15" x14ac:dyDescent="0.3">
       <c r="N183" s="19">
         <v>11.276232902933909</v>
       </c>
@@ -3413,225 +4701,654 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B78E2F1-C720-4267-9A58-0EE6E9FBFF8D}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" style="21"/>
-    <col min="3" max="4" width="13" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" style="21" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="21"/>
+    <col min="1" max="1" width="6.44140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="21"/>
+    <col min="4" max="4" width="13" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.21875" style="21" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.77734375" style="21" customWidth="1"/>
+    <col min="9" max="9" width="6.21875" style="21" customWidth="1"/>
+    <col min="10" max="16384" width="11.44140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I1" s="25"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E2" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="25"/>
+    </row>
+    <row r="3" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>72</v>
       </c>
       <c r="B3" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="E3" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="H3" s="22" t="s">
+    </row>
+    <row r="4" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="23">
+        <v>3</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="27">
+        <v>2458401.4085999997</v>
+      </c>
+      <c r="D4" s="27">
+        <f>C4-2457000</f>
+        <v>1401.4085999997333</v>
+      </c>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+    </row>
+    <row r="5" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="23">
+        <v>6</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="27">
+        <v>2458483.2110000001</v>
+      </c>
+      <c r="D5" s="27">
+        <f t="shared" ref="D5:D14" si="0">C5-2457000</f>
+        <v>1483.2110000001267</v>
+      </c>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="28">
+        <f t="shared" ref="I5:I7" si="1">C5-C4</f>
+        <v>81.802400000393391</v>
+      </c>
+      <c r="J5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+    </row>
+    <row r="6" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="23">
+        <v>9</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="27">
+        <v>2458565.0902</v>
+      </c>
+      <c r="D6" s="27">
+        <f t="shared" si="0"/>
+        <v>1565.0901999999769</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="28">
+        <f t="shared" si="1"/>
+        <v>81.879199999850243</v>
+      </c>
+      <c r="J6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+    </row>
+    <row r="7" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="23">
+        <v>12</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="27">
+        <v>2458647.3328</v>
+      </c>
+      <c r="D7" s="27">
+        <f t="shared" si="0"/>
+        <v>1647.3327999999747</v>
+      </c>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="28">
+        <f t="shared" si="1"/>
+        <v>82.242599999997765</v>
+      </c>
+      <c r="J7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="23">
+        <v>28</v>
+      </c>
+      <c r="B8" s="31" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="23">
-        <v>28</v>
-      </c>
-      <c r="B4" s="21">
-        <f>C4+2457000</f>
-        <v>2459065.2000000002</v>
-      </c>
-      <c r="C4" s="21">
-        <v>2065.1999999999998</v>
-      </c>
-      <c r="D4" s="21">
+      <c r="C8" s="27">
+        <v>2459065.2370000002</v>
+      </c>
+      <c r="D8" s="27">
+        <f t="shared" si="0"/>
+        <v>2065.2370000001974</v>
+      </c>
+      <c r="E8" s="21">
         <v>1519</v>
       </c>
-      <c r="E4" s="21">
+      <c r="F8" s="21">
         <v>1498</v>
       </c>
-      <c r="F4" s="21">
-        <f>D4-E4</f>
+      <c r="G8" s="21">
+        <f>E8-F8</f>
         <v>21</v>
       </c>
-      <c r="G4" s="24">
-        <f>F4/D4</f>
+      <c r="H8" s="24">
+        <f>G8/E8</f>
         <v>1.3824884792626729E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="23">
+      <c r="I8" s="28"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="23">
         <v>31</v>
       </c>
-      <c r="B5" s="21">
-        <f t="shared" ref="B5:B9" si="0">C5+2457000</f>
-        <v>2459148.4</v>
-      </c>
-      <c r="C5" s="21">
-        <v>2148.4</v>
-      </c>
-      <c r="D5" s="21">
+      <c r="B9" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="27">
+        <v>2459148.4781999998</v>
+      </c>
+      <c r="D9" s="27">
+        <f t="shared" si="0"/>
+        <v>2148.4781999997795</v>
+      </c>
+      <c r="E9" s="21">
         <v>1542</v>
       </c>
-      <c r="E5" s="21">
+      <c r="F9" s="21">
         <v>1520</v>
       </c>
-      <c r="F5" s="21">
-        <f t="shared" ref="F5:F7" si="1">D5-E5</f>
+      <c r="G9" s="21">
+        <f t="shared" ref="G9:G11" si="2">E9-F9</f>
         <v>22</v>
       </c>
-      <c r="G5" s="24">
-        <f t="shared" ref="G5:G7" si="2">F5/D5</f>
+      <c r="H9" s="24">
+        <f t="shared" ref="H9:H11" si="3">G9/E9</f>
         <v>1.4267185473411154E-2</v>
       </c>
-      <c r="H5" s="21">
-        <f>B5-B4</f>
-        <v>83.199999999720603</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="23">
+      <c r="I9" s="28">
+        <f>C9-C8</f>
+        <v>83.241199999582022</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="23">
         <v>34</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B10" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="27">
+        <v>2459231.1144000003</v>
+      </c>
+      <c r="D10" s="27">
         <f t="shared" si="0"/>
-        <v>2459231.1</v>
-      </c>
-      <c r="C6" s="21">
-        <v>2231.1</v>
-      </c>
-      <c r="D6" s="21">
+        <v>2231.1144000003114</v>
+      </c>
+      <c r="E10" s="21">
         <v>1472</v>
       </c>
-      <c r="E6" s="21">
+      <c r="F10" s="21">
         <v>1454</v>
       </c>
-      <c r="F6" s="21">
-        <f t="shared" si="1"/>
+      <c r="G10" s="21">
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="G6" s="24">
+      <c r="H10" s="24">
+        <f t="shared" si="3"/>
+        <v>1.2228260869565218E-2</v>
+      </c>
+      <c r="I10" s="28">
+        <f t="shared" ref="I10:I14" si="4">C10-C9</f>
+        <v>82.636200000531971</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="23">
+        <v>37</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="27">
+        <v>2459313.2535000001</v>
+      </c>
+      <c r="D11" s="27">
+        <f t="shared" si="0"/>
+        <v>2313.253500000108</v>
+      </c>
+      <c r="E11" s="21">
+        <v>1507</v>
+      </c>
+      <c r="F11" s="21">
+        <v>1488</v>
+      </c>
+      <c r="G11" s="21">
         <f t="shared" si="2"/>
-        <v>1.2228260869565218E-2</v>
-      </c>
-      <c r="H6" s="21">
-        <f t="shared" ref="H6:H7" si="3">B6-B5</f>
-        <v>82.700000000186265</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="23">
-        <v>37</v>
-      </c>
-      <c r="B7" s="21">
+        <v>19</v>
+      </c>
+      <c r="H11" s="24">
+        <f t="shared" si="3"/>
+        <v>1.2607830126078301E-2</v>
+      </c>
+      <c r="I11" s="28">
+        <f t="shared" si="4"/>
+        <v>82.139099999796599</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="23">
+        <v>61</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="27">
+        <v>2459976.0493000001</v>
+      </c>
+      <c r="D12" s="27">
         <f t="shared" si="0"/>
-        <v>2459313.2000000002</v>
-      </c>
-      <c r="C7" s="21">
-        <v>2313.1999999999998</v>
-      </c>
-      <c r="D7" s="21">
-        <v>1507</v>
-      </c>
-      <c r="E7" s="21">
-        <v>1488</v>
-      </c>
-      <c r="F7" s="21">
-        <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="G7" s="24">
-        <f t="shared" si="2"/>
-        <v>1.2607830126078301E-2</v>
-      </c>
-      <c r="H7" s="21">
-        <f t="shared" si="3"/>
-        <v>82.100000000093132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="21">
+        <v>2976.0493000000715</v>
+      </c>
+      <c r="H12" s="24"/>
+      <c r="I12" s="28"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="21">
         <v>64</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B13" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="27">
+        <v>2460059.6189000001</v>
+      </c>
+      <c r="D13" s="27">
         <f t="shared" si="0"/>
-        <v>2460059.6</v>
-      </c>
-      <c r="C8" s="21">
-        <v>3059.6</v>
-      </c>
-      <c r="D8" s="21">
+        <v>3059.6189000001177</v>
+      </c>
+      <c r="E13" s="21">
         <v>1484</v>
       </c>
-      <c r="E8" s="21">
+      <c r="F13" s="21">
         <v>1464</v>
       </c>
-      <c r="F8" s="21">
-        <f t="shared" ref="F8:F9" si="4">D8-E8</f>
+      <c r="G13" s="21">
+        <f t="shared" ref="G13:G14" si="5">E13-F13</f>
         <v>20</v>
       </c>
-      <c r="G8" s="24">
-        <f t="shared" ref="G8:G9" si="5">F8/D8</f>
+      <c r="H13" s="24">
+        <f t="shared" ref="H13:H14" si="6">G13/E13</f>
         <v>1.3477088948787063E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="21">
+      <c r="I13" s="28">
+        <f t="shared" si="4"/>
+        <v>83.569600000046194</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="21">
         <v>67</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B14" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="27">
+        <v>2460142.6048000003</v>
+      </c>
+      <c r="D14" s="27">
         <f t="shared" si="0"/>
-        <v>2460142.5</v>
-      </c>
-      <c r="C9" s="21">
-        <v>3142.5</v>
-      </c>
-      <c r="D9" s="21">
+        <v>3142.6048000003211</v>
+      </c>
+      <c r="E14" s="21">
         <v>1517</v>
       </c>
-      <c r="E9" s="21">
+      <c r="F14" s="21">
         <v>1494</v>
       </c>
-      <c r="F9" s="21">
+      <c r="G14" s="21">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="H14" s="24">
+        <f t="shared" si="6"/>
+        <v>1.5161502966381015E-2</v>
+      </c>
+      <c r="I14" s="28">
         <f t="shared" si="4"/>
-        <v>23</v>
-      </c>
-      <c r="G9" s="24">
-        <f t="shared" si="5"/>
-        <v>1.5161502966381015E-2</v>
-      </c>
-      <c r="H9" s="21">
-        <f t="shared" ref="H8:H9" si="6">B9-B8</f>
-        <v>82.899999999906868</v>
+        <v>82.985900000203401</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C18" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C19" s="33">
+        <v>2458483.2110000001</v>
+      </c>
+      <c r="D19" s="28">
+        <v>81.802400000393391</v>
+      </c>
+      <c r="E19" s="21">
+        <f>SIN((C19-$G$19)/$G$20*2*PI())*$G$22+$G$21</f>
+        <v>81.702855122563122</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="G19" s="21">
+        <v>2458740</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C20" s="33">
+        <v>2458565.0902</v>
+      </c>
+      <c r="D20" s="28">
+        <v>81.879199999850243</v>
+      </c>
+      <c r="E20" s="21">
+        <f t="shared" ref="E20:E39" si="7">SIN((C20-$G$19)/$G$20*2*PI())*$G$22+$G$21</f>
+        <v>81.7992822018347</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="G20" s="21">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C21" s="33">
+        <v>2458647.3328</v>
+      </c>
+      <c r="D21" s="28">
+        <v>82.242599999997765</v>
+      </c>
+      <c r="E21" s="21">
+        <f t="shared" si="7"/>
+        <v>82.140213815813425</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="G21" s="21">
+        <v>82.7</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C22" s="33">
+        <f>C21+83</f>
+        <v>2458730.3328</v>
+      </c>
+      <c r="D22" s="28"/>
+      <c r="E22" s="21">
+        <f t="shared" si="7"/>
+        <v>82.638059258736973</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="G22" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C23" s="33">
+        <f t="shared" ref="C23:C26" si="8">C22+83</f>
+        <v>2458813.3328</v>
+      </c>
+      <c r="D23" s="28"/>
+      <c r="E23" s="21">
+        <f t="shared" si="7"/>
+        <v>83.153035090454694</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C24" s="33">
+        <f t="shared" si="8"/>
+        <v>2458896.3328</v>
+      </c>
+      <c r="D24" s="28"/>
+      <c r="E24" s="21">
+        <f t="shared" si="7"/>
+        <v>83.542719117801852</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C25" s="33">
+        <f t="shared" si="8"/>
+        <v>2458979.3328</v>
+      </c>
+      <c r="D25" s="28"/>
+      <c r="E25" s="21">
+        <f t="shared" si="7"/>
+        <v>83.699339965118099</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C26" s="33">
+        <f t="shared" si="8"/>
+        <v>2459062.3328</v>
+      </c>
+      <c r="D26" s="28"/>
+      <c r="E26" s="21">
+        <f t="shared" si="7"/>
+        <v>83.579582425754424</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C27" s="33">
+        <v>2459148.4781999998</v>
+      </c>
+      <c r="D27" s="28">
+        <v>83.241199999582022</v>
+      </c>
+      <c r="E27" s="21">
+        <f t="shared" si="7"/>
+        <v>83.199195419955913</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C28" s="33">
+        <v>2459231.1144000003</v>
+      </c>
+      <c r="D28" s="28">
+        <v>82.636200000531971</v>
+      </c>
+      <c r="E28" s="21">
+        <f t="shared" si="7"/>
+        <v>82.692855181495872</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C29" s="33">
+        <v>2459313.2535000001</v>
+      </c>
+      <c r="D29" s="28">
+        <v>82.139099999796599</v>
+      </c>
+      <c r="E29" s="21">
+        <f t="shared" si="7"/>
+        <v>82.191215220517591</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C30" s="33">
+        <f t="shared" ref="C30:C37" si="9">C29+83</f>
+        <v>2459396.2535000001</v>
+      </c>
+      <c r="D30" s="28"/>
+      <c r="E30" s="21">
+        <f t="shared" si="7"/>
+        <v>81.824765723684834</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C31" s="33">
+        <f t="shared" si="9"/>
+        <v>2459479.2535000001</v>
+      </c>
+      <c r="D31" s="28"/>
+      <c r="E31" s="21">
+        <f t="shared" si="7"/>
+        <v>81.70037182924797</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C32" s="33">
+        <f t="shared" si="9"/>
+        <v>2459562.2535000001</v>
+      </c>
+      <c r="D32" s="28"/>
+      <c r="E32" s="21">
+        <f t="shared" si="7"/>
+        <v>81.852436027908183</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C33" s="33">
+        <f t="shared" si="9"/>
+        <v>2459645.2535000001</v>
+      </c>
+      <c r="D33" s="28"/>
+      <c r="E33" s="21">
+        <f t="shared" si="7"/>
+        <v>82.238903303990682</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C34" s="33">
+        <f t="shared" si="9"/>
+        <v>2459728.2535000001</v>
+      </c>
+      <c r="D34" s="28"/>
+      <c r="E34" s="21">
+        <f t="shared" si="7"/>
+        <v>82.752891909545326</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C35" s="33">
+        <f t="shared" si="9"/>
+        <v>2459811.2535000001</v>
+      </c>
+      <c r="D35" s="28"/>
+      <c r="E35" s="21">
+        <f t="shared" si="7"/>
+        <v>83.252252679589731</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C36" s="33">
+        <f t="shared" si="9"/>
+        <v>2459894.2535000001</v>
+      </c>
+      <c r="D36" s="28"/>
+      <c r="E36" s="21">
+        <f t="shared" si="7"/>
+        <v>83.598881936883473</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C37" s="33">
+        <f t="shared" si="9"/>
+        <v>2459977.2535000001</v>
+      </c>
+      <c r="D37" s="28"/>
+      <c r="E37" s="21">
+        <f t="shared" si="7"/>
+        <v>83.696915572864086</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C38" s="33">
+        <v>2460059.6189000001</v>
+      </c>
+      <c r="D38" s="28">
+        <v>83.569600000046194</v>
+      </c>
+      <c r="E38" s="21">
+        <f t="shared" si="7"/>
+        <v>83.521567708892789</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C39" s="33">
+        <v>2460142.6048000003</v>
+      </c>
+      <c r="D39" s="28">
+        <v>82.985900000203401</v>
+      </c>
+      <c r="E39" s="21">
+        <f t="shared" si="7"/>
+        <v>83.118777348149962</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3643,14 +5360,14 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>23</v>
       </c>
@@ -3683,7 +5400,7 @@
       <c r="AB1" s="5"/>
       <c r="AC1" s="5"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>14</v>
       </c>
@@ -3716,7 +5433,7 @@
       <c r="AB3" s="5"/>
       <c r="AC3" s="5"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -3749,7 +5466,7 @@
       <c r="AB5" s="5"/>
       <c r="AC5" s="5"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
@@ -3782,7 +5499,7 @@
       <c r="AB6" s="5"/>
       <c r="AC6" s="5"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -3815,7 +5532,7 @@
       <c r="AB7" s="5"/>
       <c r="AC7" s="5"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>18</v>
       </c>
@@ -3848,7 +5565,7 @@
       <c r="AB8" s="5"/>
       <c r="AC8" s="5"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
@@ -3881,7 +5598,7 @@
       <c r="AB9" s="5"/>
       <c r="AC9" s="5"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>20</v>
       </c>
@@ -3914,7 +5631,7 @@
       <c r="AB10" s="5"/>
       <c r="AC10" s="5"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
@@ -3947,7 +5664,7 @@
       <c r="AB11" s="5"/>
       <c r="AC11" s="5"/>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>22</v>
       </c>
@@ -3980,7 +5697,7 @@
       <c r="AB12" s="5"/>
       <c r="AC12" s="5"/>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
@@ -4013,7 +5730,7 @@
       <c r="AB14" s="5"/>
       <c r="AC14" s="5"/>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>25</v>
       </c>
@@ -4046,7 +5763,7 @@
       <c r="AB15" s="5"/>
       <c r="AC15" s="5"/>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>26</v>
       </c>
@@ -4079,7 +5796,7 @@
       <c r="AB16" s="5"/>
       <c r="AC16" s="5"/>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>27</v>
       </c>
@@ -4112,7 +5829,7 @@
       <c r="AB17" s="5"/>
       <c r="AC17" s="5"/>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>28</v>
       </c>
@@ -4145,7 +5862,7 @@
       <c r="AB18" s="5"/>
       <c r="AC18" s="5"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>29</v>
       </c>
@@ -4178,7 +5895,7 @@
       <c r="AB19" s="5"/>
       <c r="AC19" s="5"/>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>30</v>
       </c>
@@ -4211,7 +5928,7 @@
       <c r="AB20" s="5"/>
       <c r="AC20" s="5"/>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>31</v>
       </c>
@@ -4244,7 +5961,7 @@
       <c r="AB21" s="5"/>
       <c r="AC21" s="5"/>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>32</v>
       </c>
@@ -4277,7 +5994,7 @@
       <c r="AB22" s="5"/>
       <c r="AC22" s="5"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>33</v>
       </c>
@@ -4310,7 +6027,7 @@
       <c r="AB23" s="5"/>
       <c r="AC23" s="5"/>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>34</v>
       </c>
@@ -4343,7 +6060,7 @@
       <c r="AB24" s="5"/>
       <c r="AC24" s="5"/>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>35</v>
       </c>
@@ -4376,7 +6093,7 @@
       <c r="AB25" s="5"/>
       <c r="AC25" s="5"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>22</v>
       </c>
@@ -4409,7 +6126,7 @@
       <c r="AB26" s="5"/>
       <c r="AC26" s="5"/>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>0</v>
       </c>
@@ -4442,7 +6159,7 @@
       <c r="AB28" s="5"/>
       <c r="AC28" s="5"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>1</v>
       </c>
@@ -4475,7 +6192,7 @@
       <c r="AB29" s="5"/>
       <c r="AC29" s="5"/>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>2</v>
       </c>
@@ -4508,7 +6225,7 @@
       <c r="AB30" s="5"/>
       <c r="AC30" s="5"/>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>3</v>
       </c>
@@ -4541,7 +6258,7 @@
       <c r="AB31" s="5"/>
       <c r="AC31" s="5"/>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>4</v>
       </c>
@@ -4574,7 +6291,7 @@
       <c r="AB32" s="5"/>
       <c r="AC32" s="5"/>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>5</v>
       </c>
@@ -4607,7 +6324,7 @@
       <c r="AB33" s="5"/>
       <c r="AC33" s="5"/>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>6</v>
       </c>
@@ -4640,7 +6357,7 @@
       <c r="AB34" s="5"/>
       <c r="AC34" s="5"/>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>7</v>
       </c>
@@ -4673,7 +6390,7 @@
       <c r="AB35" s="5"/>
       <c r="AC35" s="5"/>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>8</v>
       </c>
@@ -4706,7 +6423,7 @@
       <c r="AB36" s="5"/>
       <c r="AC36" s="5"/>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>9</v>
       </c>
@@ -4739,7 +6456,7 @@
       <c r="AB37" s="5"/>
       <c r="AC37" s="5"/>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>10</v>
       </c>
@@ -4772,7 +6489,7 @@
       <c r="AB38" s="5"/>
       <c r="AC38" s="5"/>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
         <v>11</v>
       </c>
@@ -4805,7 +6522,7 @@
       <c r="AB39" s="5"/>
       <c r="AC39" s="5"/>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
         <v>12</v>
       </c>
@@ -4838,7 +6555,7 @@
       <c r="AB40" s="5"/>
       <c r="AC40" s="5"/>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
         <v>13</v>
       </c>
@@ -4871,12 +6588,12 @@
       <c r="AB41" s="5"/>
       <c r="AC41" s="5"/>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A43" s="16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>39</v>
       </c>
@@ -4887,7 +6604,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>41</v>
       </c>
@@ -4900,7 +6617,7 @@
       <c r="D45" s="1"/>
       <c r="F45" s="1"/>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>36</v>
       </c>
@@ -4912,7 +6629,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>38</v>
       </c>
@@ -4930,7 +6647,7 @@
         <v>0.1740000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>40</v>
       </c>
@@ -4941,7 +6658,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
0.3.7 result output enhancements
</commit_message>
<xml_diff>
--- a/research/star_systems/TOI-4504/TOI-4504.xlsx
+++ b/research/star_systems/TOI-4504/TOI-4504.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meine Ablage\Python\curvesim\research\star_systems\TOI-4504\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1588426E-07FC-4D54-93E4-BAC9F0FF17BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B973BA79-592B-4777-87CF-EA978CAADDAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{6919DDE8-15F9-45FB-B5F7-4209377AF865}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{6919DDE8-15F9-45FB-B5F7-4209377AF865}"/>
   </bookViews>
   <sheets>
     <sheet name="Planet c" sheetId="5" r:id="rId1"/>
@@ -2100,7 +2100,7 @@
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2241,6 +2241,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2284,7 +2290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2373,6 +2379,8 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -10147,7 +10155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{297EEAD8-1435-4033-9511-E3E1B196AAA2}">
   <dimension ref="A1:O183"/>
   <sheetViews>
-    <sheetView topLeftCell="A154" workbookViewId="0">
+    <sheetView topLeftCell="A142" workbookViewId="0">
       <selection activeCell="K189" sqref="K189"/>
     </sheetView>
   </sheetViews>
@@ -10361,7 +10369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B78E2F1-C720-4267-9A58-0EE6E9FBFF8D}">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -11015,7 +11023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5275C9A-EF05-481E-A9DC-3AD994004FAC}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
@@ -11993,9 +12001,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB98D226-8F0E-4E9D-B925-EBA798192E0A}">
   <dimension ref="A1:P129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12085,6 +12093,9 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="42">
+        <v>42981</v>
+      </c>
       <c r="B5" s="21">
         <v>3</v>
       </c>
@@ -12101,13 +12112,20 @@
         <v>82.115313636718767</v>
       </c>
       <c r="H5" s="38"/>
-      <c r="I5" s="39"/>
+      <c r="I5" s="39">
+        <f>2461150</f>
+        <v>2461150</v>
+      </c>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
       <c r="L5" s="39"/>
       <c r="M5" s="39"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="42">
+        <f>D6-$D$5+$A$5</f>
+        <v>43062.802400000393</v>
+      </c>
       <c r="B6" s="23">
         <v>6</v>
       </c>
@@ -12123,17 +12141,24 @@
       </c>
       <c r="F6" s="39"/>
       <c r="G6" s="38">
-        <f t="shared" ref="G6:H69" si="0">SIN(($D6-$P$1)/$P$2*2*PI())*$P$4+$P$3</f>
+        <f t="shared" ref="G6:G69" si="0">SIN(($D6-$P$1)/$P$2*2*PI())*$P$4+$P$3</f>
         <v>81.908126674215765</v>
       </c>
       <c r="H6" s="38"/>
-      <c r="I6" s="39"/>
+      <c r="I6" s="38">
+        <f>I5-D5</f>
+        <v>2748.5914000002667</v>
+      </c>
       <c r="J6" s="39"/>
       <c r="K6" s="39"/>
       <c r="L6" s="39"/>
       <c r="M6" s="39"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="42">
+        <f t="shared" ref="A7:A70" si="1">D7-$D$5+$A$5</f>
+        <v>43144.681600000244</v>
+      </c>
       <c r="B7" s="21">
         <v>9</v>
       </c>
@@ -12144,7 +12169,7 @@
         <v>2458565.0902</v>
       </c>
       <c r="E7" s="38">
-        <f t="shared" ref="E7:E15" si="1">D7-D6</f>
+        <f t="shared" ref="E7:E15" si="2">D7-D6</f>
         <v>81.879199999850243</v>
       </c>
       <c r="F7" s="39"/>
@@ -12160,6 +12185,10 @@
       <c r="M7" s="39"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="42">
+        <f t="shared" si="1"/>
+        <v>43226.924200000241</v>
+      </c>
       <c r="B8" s="23">
         <v>12</v>
       </c>
@@ -12170,7 +12199,7 @@
         <v>2458647.3328</v>
       </c>
       <c r="E8" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>82.242599999997765</v>
       </c>
       <c r="F8" s="39"/>
@@ -12186,6 +12215,10 @@
       <c r="M8" s="39"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="42">
+        <f t="shared" si="1"/>
+        <v>43644.828400000464</v>
+      </c>
       <c r="B9" s="21">
         <v>28</v>
       </c>
@@ -12206,6 +12239,10 @@
       <c r="M9" s="39"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="42">
+        <f t="shared" si="1"/>
+        <v>43728.069600000046</v>
+      </c>
       <c r="B10" s="21">
         <v>31</v>
       </c>
@@ -12216,7 +12253,7 @@
         <v>2459148.4781999998</v>
       </c>
       <c r="E10" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>83.241199999582022</v>
       </c>
       <c r="F10" s="39"/>
@@ -12232,6 +12269,10 @@
       <c r="M10" s="39"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="42">
+        <f t="shared" si="1"/>
+        <v>43810.705800000578</v>
+      </c>
       <c r="B11" s="23">
         <v>34</v>
       </c>
@@ -12242,7 +12283,7 @@
         <v>2459231.1144000003</v>
       </c>
       <c r="E11" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>82.636200000531971</v>
       </c>
       <c r="F11" s="39"/>
@@ -12258,6 +12299,10 @@
       <c r="M11" s="39"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="42">
+        <f t="shared" si="1"/>
+        <v>43892.844900000375</v>
+      </c>
       <c r="B12" s="21">
         <v>37</v>
       </c>
@@ -12268,7 +12313,7 @@
         <v>2459313.2535000001</v>
       </c>
       <c r="E12" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>82.139099999796599</v>
       </c>
       <c r="F12" s="40"/>
@@ -12284,6 +12329,10 @@
       <c r="M12" s="39"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="42">
+        <f t="shared" si="1"/>
+        <v>44555.640700000338</v>
+      </c>
       <c r="B13" s="21">
         <v>61</v>
       </c>
@@ -12304,6 +12353,10 @@
       <c r="M13" s="39"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="42">
+        <f t="shared" si="1"/>
+        <v>44639.210300000384</v>
+      </c>
       <c r="B14" s="23">
         <v>64</v>
       </c>
@@ -12314,7 +12367,7 @@
         <v>2460059.6189000001</v>
       </c>
       <c r="E14" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>83.569600000046194</v>
       </c>
       <c r="F14" s="39"/>
@@ -12330,6 +12383,10 @@
       <c r="M14" s="39"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="42">
+        <f t="shared" si="1"/>
+        <v>44722.196200000588</v>
+      </c>
       <c r="B15" s="21">
         <v>67</v>
       </c>
@@ -12340,7 +12397,7 @@
         <v>2460142.6048000003</v>
       </c>
       <c r="E15" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>82.985900000203401</v>
       </c>
       <c r="F15" s="40"/>
@@ -12356,6 +12413,10 @@
       <c r="M15" s="39"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="42">
+        <f t="shared" si="1"/>
+        <v>42981.000000000466</v>
+      </c>
       <c r="D16" s="38">
         <v>2458401.4086000002</v>
       </c>
@@ -12369,7 +12430,11 @@
       <c r="L16" s="39"/>
       <c r="M16" s="39"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="42">
+        <f t="shared" si="1"/>
+        <v>43062.814500000328</v>
+      </c>
       <c r="D17" s="38">
         <v>2458483.2231000001</v>
       </c>
@@ -12389,13 +12454,17 @@
       <c r="L17" s="39"/>
       <c r="M17" s="39"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="42">
+        <f t="shared" si="1"/>
+        <v>43144.698700000066</v>
+      </c>
       <c r="D18" s="38">
         <v>2458565.1072999998</v>
       </c>
       <c r="E18" s="39"/>
       <c r="F18" s="40">
-        <f t="shared" ref="F18:F81" si="2">D18-D17</f>
+        <f t="shared" ref="F18:F81" si="3">D18-D17</f>
         <v>81.884199999738485</v>
       </c>
       <c r="G18" s="38">
@@ -12409,13 +12478,17 @@
       <c r="L18" s="39"/>
       <c r="M18" s="39"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="42">
+        <f t="shared" si="1"/>
+        <v>43226.954900000244</v>
+      </c>
       <c r="D19" s="38">
         <v>2458647.3635</v>
       </c>
       <c r="E19" s="39"/>
       <c r="F19" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.256200000178069</v>
       </c>
       <c r="G19" s="38">
@@ -12429,13 +12502,17 @@
       <c r="L19" s="39"/>
       <c r="M19" s="39"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="42">
+        <f t="shared" si="1"/>
+        <v>43309.847800000105</v>
+      </c>
       <c r="D20" s="38">
         <v>2458730.2563999998</v>
       </c>
       <c r="E20" s="39"/>
       <c r="F20" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.892899999860674</v>
       </c>
       <c r="G20" s="38">
@@ -12449,13 +12526,17 @@
       <c r="L20" s="39"/>
       <c r="M20" s="39"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="42">
+        <f t="shared" si="1"/>
+        <v>43393.384000000078</v>
+      </c>
       <c r="D21" s="38">
         <v>2458813.7925999998</v>
       </c>
       <c r="E21" s="39"/>
       <c r="F21" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.536199999973178</v>
       </c>
       <c r="G21" s="38">
@@ -12469,13 +12550,17 @@
       <c r="L21" s="39"/>
       <c r="M21" s="39"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="42">
+        <f t="shared" si="1"/>
+        <v>43477.251600000076</v>
+      </c>
       <c r="D22" s="38">
         <v>2458897.6601999998</v>
       </c>
       <c r="E22" s="39"/>
       <c r="F22" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.867599999997765</v>
       </c>
       <c r="G22" s="38">
@@ -12489,13 +12574,17 @@
       <c r="L22" s="39"/>
       <c r="M22" s="39"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="42">
+        <f t="shared" si="1"/>
+        <v>43561.156600000337</v>
+      </c>
       <c r="D23" s="38">
         <v>2458981.5652000001</v>
       </c>
       <c r="E23" s="39"/>
       <c r="F23" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.90500000026077</v>
       </c>
       <c r="G23" s="38">
@@ -12509,13 +12598,17 @@
       <c r="L23" s="39"/>
       <c r="M23" s="39"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="42">
+        <f t="shared" si="1"/>
+        <v>43644.853600000497</v>
+      </c>
       <c r="D24" s="38">
         <v>2459065.2622000002</v>
       </c>
       <c r="E24" s="39"/>
       <c r="F24" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.697000000160187</v>
       </c>
       <c r="G24" s="38">
@@ -12529,7 +12622,11 @@
       <c r="L24" s="39"/>
       <c r="M24" s="39"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="42">
+        <f t="shared" si="1"/>
+        <v>43728.083100000396</v>
+      </c>
       <c r="B25" s="23"/>
       <c r="C25" s="31"/>
       <c r="D25" s="38">
@@ -12537,7 +12634,7 @@
       </c>
       <c r="E25" s="40"/>
       <c r="F25" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.229499999899417</v>
       </c>
       <c r="G25" s="38">
@@ -12551,13 +12648,17 @@
       <c r="L25" s="39"/>
       <c r="M25" s="39"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="42">
+        <f t="shared" si="1"/>
+        <v>43810.712000000291</v>
+      </c>
       <c r="D26" s="38">
         <v>2459231.1206</v>
       </c>
       <c r="E26" s="39"/>
       <c r="F26" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.628899999894202</v>
       </c>
       <c r="G26" s="38">
@@ -12571,13 +12672,17 @@
       <c r="L26" s="39"/>
       <c r="M26" s="39"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="42">
+        <f t="shared" si="1"/>
+        <v>43892.846600000281</v>
+      </c>
       <c r="D27" s="38">
         <v>2459313.2552</v>
       </c>
       <c r="E27" s="39"/>
       <c r="F27" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.134599999990314</v>
       </c>
       <c r="G27" s="38">
@@ -12591,7 +12696,11 @@
       <c r="L27" s="39"/>
       <c r="M27" s="39"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="42">
+        <f t="shared" si="1"/>
+        <v>43974.720100000035</v>
+      </c>
       <c r="B28" s="23"/>
       <c r="C28" s="31"/>
       <c r="D28" s="38">
@@ -12599,7 +12708,7 @@
       </c>
       <c r="E28" s="40"/>
       <c r="F28" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>81.873499999754131</v>
       </c>
       <c r="G28" s="38">
@@ -12613,13 +12722,17 @@
       <c r="L28" s="39"/>
       <c r="M28" s="39"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="42">
+        <f t="shared" si="1"/>
+        <v>44056.568500000052</v>
+      </c>
       <c r="D29" s="38">
         <v>2459476.9770999998</v>
       </c>
       <c r="E29" s="39"/>
       <c r="F29" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>81.848400000017136</v>
       </c>
       <c r="G29" s="38">
@@ -12633,13 +12746,17 @@
       <c r="L29" s="39"/>
       <c r="M29" s="39"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="42">
+        <f t="shared" si="1"/>
+        <v>44138.62200000044</v>
+      </c>
       <c r="D30" s="38">
         <v>2459559.0306000002</v>
       </c>
       <c r="E30" s="39"/>
       <c r="F30" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.05350000038743</v>
       </c>
       <c r="G30" s="38">
@@ -12653,7 +12770,11 @@
       <c r="L30" s="39"/>
       <c r="M30" s="39"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="42">
+        <f t="shared" si="1"/>
+        <v>44221.118600000162</v>
+      </c>
       <c r="B31" s="23"/>
       <c r="C31" s="31"/>
       <c r="D31" s="38">
@@ -12661,7 +12782,7 @@
       </c>
       <c r="E31" s="40"/>
       <c r="F31" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.496599999722093</v>
       </c>
       <c r="G31" s="38">
@@ -12675,13 +12796,17 @@
       <c r="L31" s="39"/>
       <c r="M31" s="39"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="42">
+        <f t="shared" si="1"/>
+        <v>44304.222000000067</v>
+      </c>
       <c r="D32" s="38">
         <v>2459724.6305999998</v>
       </c>
       <c r="E32" s="39"/>
       <c r="F32" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.103399999905378</v>
       </c>
       <c r="G32" s="38">
@@ -12695,13 +12820,17 @@
       <c r="L32" s="39"/>
       <c r="M32" s="39"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="42">
+        <f t="shared" si="1"/>
+        <v>44387.864700000267</v>
+      </c>
       <c r="D33" s="38">
         <v>2459808.2733</v>
       </c>
       <c r="E33" s="39"/>
       <c r="F33" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.642700000200421</v>
       </c>
       <c r="G33" s="38">
@@ -12715,7 +12844,11 @@
       <c r="L33" s="39"/>
       <c r="M33" s="39"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="42">
+        <f t="shared" si="1"/>
+        <v>44471.776000000071</v>
+      </c>
       <c r="B34" s="23"/>
       <c r="C34" s="31"/>
       <c r="D34" s="38">
@@ -12723,7 +12856,7 @@
       </c>
       <c r="E34" s="40"/>
       <c r="F34" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.911299999803305</v>
       </c>
       <c r="G34" s="38">
@@ -12739,13 +12872,17 @@
       <c r="L34" s="39"/>
       <c r="M34" s="39"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="42">
+        <f t="shared" si="1"/>
+        <v>44555.658500000369</v>
+      </c>
       <c r="D35" s="38">
         <v>2459976.0671000001</v>
       </c>
       <c r="E35" s="39"/>
       <c r="F35" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.882500000298023</v>
       </c>
       <c r="G35" s="38">
@@ -12759,13 +12896,17 @@
       <c r="L35" s="39"/>
       <c r="M35" s="39"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="42">
+        <f t="shared" si="1"/>
+        <v>44639.209800000302</v>
+      </c>
       <c r="D36" s="38">
         <v>2460059.6184</v>
       </c>
       <c r="E36" s="39"/>
       <c r="F36" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.55129999993369</v>
       </c>
       <c r="G36" s="38">
@@ -12779,13 +12920,17 @@
       <c r="L36" s="39"/>
       <c r="M36" s="39"/>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="42">
+        <f t="shared" si="1"/>
+        <v>44722.18450000044</v>
+      </c>
       <c r="D37" s="38">
         <v>2460142.5931000002</v>
       </c>
       <c r="E37" s="39"/>
       <c r="F37" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.974700000137091</v>
       </c>
       <c r="G37" s="38">
@@ -12799,13 +12944,17 @@
       <c r="L37" s="39"/>
       <c r="M37" s="39"/>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="42">
+        <f t="shared" si="1"/>
+        <v>44804.572600000072</v>
+      </c>
       <c r="D38" s="38">
         <v>2460224.9811999998</v>
       </c>
       <c r="E38" s="39"/>
       <c r="F38" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.388099999632686</v>
       </c>
       <c r="G38" s="38">
@@ -12819,13 +12968,17 @@
       <c r="L38" s="39"/>
       <c r="M38" s="39"/>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="42">
+        <f t="shared" si="1"/>
+        <v>44886.571600000374</v>
+      </c>
       <c r="D39" s="38">
         <v>2460306.9802000001</v>
       </c>
       <c r="E39" s="39"/>
       <c r="F39" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>81.999000000301749</v>
       </c>
       <c r="G39" s="38">
@@ -12839,13 +12992,17 @@
       <c r="L39" s="39"/>
       <c r="M39" s="39"/>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="42">
+        <f t="shared" si="1"/>
+        <v>44968.432900000364</v>
+      </c>
       <c r="D40" s="38">
         <v>2460388.8415000001</v>
       </c>
       <c r="E40" s="39"/>
       <c r="F40" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>81.861299999989569</v>
       </c>
       <c r="G40" s="38">
@@ -12859,13 +13016,17 @@
       <c r="L40" s="39"/>
       <c r="M40" s="39"/>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="42">
+        <f t="shared" si="1"/>
+        <v>45050.412800000049</v>
+      </c>
       <c r="D41" s="38">
         <v>2460470.8213999998</v>
       </c>
       <c r="E41" s="39"/>
       <c r="F41" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>81.979899999685585</v>
       </c>
       <c r="G41" s="38">
@@ -12879,13 +13040,17 @@
       <c r="L41" s="39"/>
       <c r="M41" s="39"/>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="42">
+        <f t="shared" si="1"/>
+        <v>45132.771900000051</v>
+      </c>
       <c r="D42" s="38">
         <v>2460553.1804999998</v>
       </c>
       <c r="E42" s="39"/>
       <c r="F42" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.35910000000149</v>
       </c>
       <c r="G42" s="38">
@@ -12899,13 +13064,17 @@
       <c r="L42" s="39"/>
       <c r="M42" s="39"/>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="42">
+        <f t="shared" si="1"/>
+        <v>45215.699500000104</v>
+      </c>
       <c r="D43" s="38">
         <v>2460636.1080999998</v>
       </c>
       <c r="E43" s="39"/>
       <c r="F43" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.927600000053644</v>
       </c>
       <c r="G43" s="38">
@@ -12919,13 +13088,17 @@
       <c r="L43" s="39"/>
       <c r="M43" s="39"/>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="42">
+        <f t="shared" si="1"/>
+        <v>45299.183400000446</v>
+      </c>
       <c r="D44" s="38">
         <v>2460719.5920000002</v>
       </c>
       <c r="E44" s="39"/>
       <c r="F44" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.483900000341237</v>
       </c>
       <c r="G44" s="38">
@@ -12939,13 +13112,17 @@
       <c r="L44" s="39"/>
       <c r="M44" s="39"/>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="42">
+        <f t="shared" si="1"/>
+        <v>45383.01630000025</v>
+      </c>
       <c r="D45" s="38">
         <v>2460803.4249</v>
       </c>
       <c r="E45" s="39"/>
       <c r="F45" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.832899999804795</v>
       </c>
       <c r="G45" s="38">
@@ -12959,13 +13136,17 @@
       <c r="L45" s="39"/>
       <c r="M45" s="39"/>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="42">
+        <f t="shared" si="1"/>
+        <v>45466.910600000061</v>
+      </c>
       <c r="D46" s="38">
         <v>2460887.3191999998</v>
       </c>
       <c r="E46" s="39"/>
       <c r="F46" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.894299999810755</v>
       </c>
       <c r="G46" s="38">
@@ -12979,13 +13160,17 @@
       <c r="L46" s="39"/>
       <c r="M46" s="39"/>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="42">
+        <f t="shared" si="1"/>
+        <v>45550.570000000298</v>
+      </c>
       <c r="D47" s="38">
         <v>2460970.9786</v>
       </c>
       <c r="E47" s="39"/>
       <c r="F47" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.659400000236928</v>
       </c>
       <c r="G47" s="38">
@@ -12999,13 +13184,17 @@
       <c r="L47" s="39"/>
       <c r="M47" s="39"/>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="42">
+        <f t="shared" si="1"/>
+        <v>45633.725600000471</v>
+      </c>
       <c r="D48" s="38">
         <v>2461054.1342000002</v>
       </c>
       <c r="E48" s="39"/>
       <c r="F48" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.155600000172853</v>
       </c>
       <c r="G48" s="38">
@@ -13019,13 +13208,17 @@
       <c r="L48" s="39"/>
       <c r="M48" s="39"/>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="43">
+        <f t="shared" si="1"/>
+        <v>45716.270100000314</v>
+      </c>
       <c r="D49" s="38">
         <v>2461136.6787</v>
       </c>
       <c r="E49" s="39"/>
       <c r="F49" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.544499999843538</v>
       </c>
       <c r="G49" s="38">
@@ -13039,13 +13232,17 @@
       <c r="L49" s="39"/>
       <c r="M49" s="39"/>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="42">
+        <f t="shared" si="1"/>
+        <v>45798.352500000037</v>
+      </c>
       <c r="D50" s="38">
         <v>2461218.7610999998</v>
       </c>
       <c r="E50" s="39"/>
       <c r="F50" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.082399999722838</v>
       </c>
       <c r="G50" s="38">
@@ -13059,7 +13256,11 @@
       <c r="L50" s="39"/>
       <c r="M50" s="39"/>
     </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="42">
+        <f t="shared" si="1"/>
+        <v>45880.264500000048</v>
+      </c>
       <c r="B51" s="23"/>
       <c r="C51" s="31"/>
       <c r="D51" s="38">
@@ -13067,7 +13268,7 @@
       </c>
       <c r="E51" s="40"/>
       <c r="F51" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>81.912000000011176</v>
       </c>
       <c r="G51" s="38">
@@ -13081,13 +13282,17 @@
       <c r="L51" s="39"/>
       <c r="M51" s="39"/>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="42">
+        <f t="shared" si="1"/>
+        <v>45962.332100000232</v>
+      </c>
       <c r="D52" s="38">
         <v>2461382.7407</v>
       </c>
       <c r="E52" s="39"/>
       <c r="F52" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.067600000184029</v>
       </c>
       <c r="G52" s="38">
@@ -13101,13 +13306,17 @@
       <c r="L52" s="39"/>
       <c r="M52" s="39"/>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="42">
+        <f t="shared" si="1"/>
+        <v>46044.858300000429</v>
+      </c>
       <c r="D53" s="38">
         <v>2461465.2669000002</v>
       </c>
       <c r="E53" s="39"/>
       <c r="F53" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.526200000196695</v>
       </c>
       <c r="G53" s="38">
@@ -13115,19 +13324,23 @@
         <v>82.165472802482711</v>
       </c>
       <c r="H53" s="38"/>
-      <c r="I53" s="39"/>
+      <c r="I53" s="38"/>
       <c r="J53" s="39"/>
       <c r="K53" s="39"/>
       <c r="L53" s="39"/>
       <c r="M53" s="39"/>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="42">
+        <f t="shared" si="1"/>
+        <v>46127.976500000339</v>
+      </c>
       <c r="D54" s="38">
         <v>2461548.3851000001</v>
       </c>
       <c r="E54" s="39"/>
       <c r="F54" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.118199999909848</v>
       </c>
       <c r="G54" s="38">
@@ -13141,14 +13354,18 @@
       <c r="L54" s="39"/>
       <c r="M54" s="39"/>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="42">
+        <f t="shared" si="1"/>
+        <v>46211.551400000229</v>
+      </c>
       <c r="C55" s="32"/>
       <c r="D55" s="38">
         <v>2461631.96</v>
       </c>
       <c r="E55" s="40"/>
       <c r="F55" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.574899999890476</v>
       </c>
       <c r="G55" s="38">
@@ -13162,13 +13379,17 @@
       <c r="L55" s="39"/>
       <c r="M55" s="39"/>
     </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="42">
+        <f t="shared" si="1"/>
+        <v>46295.357400000095</v>
+      </c>
       <c r="D56" s="38">
         <v>2461715.7659999998</v>
       </c>
       <c r="E56" s="39"/>
       <c r="F56" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.80599999986589</v>
       </c>
       <c r="G56" s="38">
@@ -13182,13 +13403,17 @@
       <c r="L56" s="39"/>
       <c r="M56" s="39"/>
     </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="42">
+        <f t="shared" si="1"/>
+        <v>46379.180700000376</v>
+      </c>
       <c r="D57" s="38">
         <v>2461799.5893000001</v>
       </c>
       <c r="E57" s="39"/>
       <c r="F57" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.823300000280142</v>
       </c>
       <c r="G57" s="38">
@@ -13202,14 +13427,18 @@
       <c r="L57" s="39"/>
       <c r="M57" s="39"/>
     </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="42">
+        <f t="shared" si="1"/>
+        <v>46462.773600000422</v>
+      </c>
       <c r="C58" s="32"/>
       <c r="D58" s="38">
         <v>2461883.1822000002</v>
       </c>
       <c r="E58" s="40"/>
       <c r="F58" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.592900000046939</v>
       </c>
       <c r="G58" s="38">
@@ -13223,13 +13452,17 @@
       <c r="L58" s="39"/>
       <c r="M58" s="39"/>
     </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="42">
+        <f t="shared" si="1"/>
+        <v>46545.879400000442</v>
+      </c>
       <c r="D59" s="38">
         <v>2461966.2880000002</v>
       </c>
       <c r="E59" s="39"/>
       <c r="F59" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.105800000019372</v>
       </c>
       <c r="G59" s="38">
@@ -13243,13 +13476,17 @@
       <c r="L59" s="39"/>
       <c r="M59" s="39"/>
     </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="42">
+        <f t="shared" si="1"/>
+        <v>46628.393000000156</v>
+      </c>
       <c r="D60" s="38">
         <v>2462048.8015999999</v>
       </c>
       <c r="E60" s="39"/>
       <c r="F60" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.513599999714643</v>
       </c>
       <c r="G60" s="38">
@@ -13263,13 +13500,17 @@
       <c r="L60" s="39"/>
       <c r="M60" s="39"/>
     </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="42">
+        <f t="shared" si="1"/>
+        <v>46710.452000000048</v>
+      </c>
       <c r="D61" s="38">
         <v>2462130.8605999998</v>
       </c>
       <c r="E61" s="39"/>
       <c r="F61" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.058999999891967</v>
       </c>
       <c r="G61" s="38">
@@ -13283,13 +13524,17 @@
       <c r="L61" s="39"/>
       <c r="M61" s="39"/>
     </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" s="42">
+        <f t="shared" si="1"/>
+        <v>46792.322300000116</v>
+      </c>
       <c r="D62" s="38">
         <v>2462212.7308999998</v>
       </c>
       <c r="E62" s="39"/>
       <c r="F62" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>81.8703000000678</v>
       </c>
       <c r="G62" s="38">
@@ -13303,13 +13548,17 @@
       <c r="L62" s="39"/>
       <c r="M62" s="39"/>
     </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="42">
+        <f t="shared" si="1"/>
+        <v>46874.286100000143</v>
+      </c>
       <c r="D63" s="38">
         <v>2462294.6946999999</v>
       </c>
       <c r="E63" s="39"/>
       <c r="F63" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>81.963800000026822</v>
       </c>
       <c r="G63" s="38">
@@ -13323,13 +13572,17 @@
       <c r="L63" s="39"/>
       <c r="M63" s="39"/>
     </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="42">
+        <f t="shared" si="1"/>
+        <v>46956.619700000156</v>
+      </c>
       <c r="D64" s="38">
         <v>2462377.0282999999</v>
       </c>
       <c r="E64" s="39"/>
       <c r="F64" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.333600000012666</v>
       </c>
       <c r="G64" s="38">
@@ -13343,13 +13596,17 @@
       <c r="L64" s="39"/>
       <c r="M64" s="39"/>
     </row>
-    <row r="65" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" s="42">
+        <f t="shared" si="1"/>
+        <v>47039.537700000219</v>
+      </c>
       <c r="D65" s="38">
         <v>2462459.9463</v>
       </c>
       <c r="E65" s="39"/>
       <c r="F65" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.91800000006333</v>
       </c>
       <c r="G65" s="38">
@@ -13363,13 +13620,17 @@
       <c r="L65" s="39"/>
       <c r="M65" s="39"/>
     </row>
-    <row r="66" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" s="42">
+        <f t="shared" si="1"/>
+        <v>47123.037000000477</v>
+      </c>
       <c r="D66" s="38">
         <v>2462543.4456000002</v>
       </c>
       <c r="E66" s="39"/>
       <c r="F66" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.49930000025779</v>
       </c>
       <c r="G66" s="38">
@@ -13383,13 +13644,17 @@
       <c r="L66" s="39"/>
       <c r="M66" s="39"/>
     </row>
-    <row r="67" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" s="42">
+        <f t="shared" si="1"/>
+        <v>47206.87060000049</v>
+      </c>
       <c r="D67" s="38">
         <v>2462627.2792000002</v>
       </c>
       <c r="E67" s="39"/>
       <c r="F67" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.833600000012666</v>
       </c>
       <c r="G67" s="38">
@@ -13403,13 +13668,17 @@
       <c r="L67" s="39"/>
       <c r="M67" s="39"/>
     </row>
-    <row r="68" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" s="42">
+        <f t="shared" si="1"/>
+        <v>47290.727500000037</v>
+      </c>
       <c r="D68" s="38">
         <v>2462711.1360999998</v>
       </c>
       <c r="E68" s="39"/>
       <c r="F68" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.85689999954775</v>
       </c>
       <c r="G68" s="38">
@@ -13423,13 +13692,17 @@
       <c r="L68" s="39"/>
       <c r="M68" s="39"/>
     </row>
-    <row r="69" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" s="42">
+        <f t="shared" si="1"/>
+        <v>47374.343800000381</v>
+      </c>
       <c r="D69" s="38">
         <v>2462794.7524000001</v>
       </c>
       <c r="E69" s="39"/>
       <c r="F69" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.616300000343472</v>
       </c>
       <c r="G69" s="38">
@@ -13443,17 +13716,21 @@
       <c r="L69" s="39"/>
       <c r="M69" s="39"/>
     </row>
-    <row r="70" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" s="42">
+        <f t="shared" si="1"/>
+        <v>47457.502300000284</v>
+      </c>
       <c r="D70" s="38">
         <v>2462877.9109</v>
       </c>
       <c r="E70" s="39"/>
       <c r="F70" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.158499999903142</v>
       </c>
       <c r="G70" s="38">
-        <f t="shared" ref="G70:H95" si="3">SIN(($D70-$P$1)/$P$2*2*PI())*$P$4+$P$3</f>
+        <f t="shared" ref="G70:G95" si="4">SIN(($D70-$P$1)/$P$2*2*PI())*$P$4+$P$3</f>
         <v>83.687468386446824</v>
       </c>
       <c r="H70" s="38"/>
@@ -13463,17 +13740,21 @@
       <c r="L70" s="39"/>
       <c r="M70" s="39"/>
     </row>
-    <row r="71" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" s="42">
+        <f t="shared" ref="A71:A122" si="5">D71-$D$5+$A$5</f>
+        <v>47540.114400000311</v>
+      </c>
       <c r="D71" s="38">
         <v>2462960.523</v>
       </c>
       <c r="E71" s="39"/>
       <c r="F71" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.612100000027567</v>
       </c>
       <c r="G71" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>83.252559011328415</v>
       </c>
       <c r="H71" s="38"/>
@@ -13483,17 +13764,21 @@
       <c r="L71" s="39"/>
       <c r="M71" s="39"/>
     </row>
-    <row r="72" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" s="42">
+        <f t="shared" si="5"/>
+        <v>47622.275900000241</v>
+      </c>
       <c r="D72" s="38">
         <v>2463042.6845</v>
       </c>
       <c r="E72" s="39"/>
       <c r="F72" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.161499999929219</v>
       </c>
       <c r="G72" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>82.717919468018579</v>
       </c>
       <c r="H72" s="38"/>
@@ -13503,17 +13788,21 @@
       <c r="L72" s="39"/>
       <c r="M72" s="39"/>
     </row>
-    <row r="73" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" s="42">
+        <f t="shared" si="5"/>
+        <v>47704.188100000378</v>
+      </c>
       <c r="D73" s="38">
         <v>2463124.5967000001</v>
       </c>
       <c r="E73" s="39"/>
       <c r="F73" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>81.912200000137091</v>
       </c>
       <c r="G73" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>82.236969846126186</v>
       </c>
       <c r="H73" s="38"/>
@@ -13523,17 +13812,21 @@
       <c r="L73" s="39"/>
       <c r="M73" s="39"/>
     </row>
-    <row r="74" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" s="42">
+        <f t="shared" si="5"/>
+        <v>47786.075100000482</v>
+      </c>
       <c r="D74" s="38">
         <v>2463206.4837000002</v>
       </c>
       <c r="E74" s="39"/>
       <c r="F74" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>81.887000000104308</v>
       </c>
       <c r="G74" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>81.945956935419034</v>
       </c>
       <c r="H74" s="38"/>
@@ -13543,17 +13836,21 @@
       <c r="L74" s="39"/>
       <c r="M74" s="39"/>
     </row>
-    <row r="75" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" s="42">
+        <f t="shared" si="5"/>
+        <v>47868.166100000497</v>
+      </c>
       <c r="D75" s="38">
         <v>2463288.5747000002</v>
       </c>
       <c r="E75" s="39"/>
       <c r="F75" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.091000000014901</v>
       </c>
       <c r="G75" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>81.928328707040492</v>
       </c>
       <c r="H75" s="38"/>
@@ -13563,17 +13860,21 @@
       <c r="L75" s="39"/>
       <c r="M75" s="39"/>
     </row>
-    <row r="76" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76" s="42">
+        <f t="shared" si="5"/>
+        <v>47950.682300000452</v>
+      </c>
       <c r="D76" s="38">
         <v>2463371.0909000002</v>
       </c>
       <c r="E76" s="39"/>
       <c r="F76" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.516199999954551</v>
       </c>
       <c r="G76" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>82.192149544455901</v>
       </c>
       <c r="H76" s="38"/>
@@ -13583,17 +13884,21 @@
       <c r="L76" s="39"/>
       <c r="M76" s="39"/>
     </row>
-    <row r="77" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77" s="42">
+        <f t="shared" si="5"/>
+        <v>48033.757700000424</v>
+      </c>
       <c r="D77" s="38">
         <v>2463454.1663000002</v>
       </c>
       <c r="E77" s="39"/>
       <c r="F77" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.075399999972433</v>
       </c>
       <c r="G77" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>82.665212680613806</v>
       </c>
       <c r="H77" s="38"/>
@@ -13603,17 +13908,21 @@
       <c r="L77" s="39"/>
       <c r="M77" s="39"/>
     </row>
-    <row r="78" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78" s="42">
+        <f t="shared" si="5"/>
+        <v>48117.334800000302</v>
+      </c>
       <c r="D78" s="38">
         <v>2463537.7434</v>
       </c>
       <c r="E78" s="39"/>
       <c r="F78" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.577099999878556</v>
       </c>
       <c r="G78" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>83.210547621405894</v>
       </c>
       <c r="H78" s="38"/>
@@ -13623,17 +13932,21 @@
       <c r="L78" s="39"/>
       <c r="M78" s="39"/>
     </row>
-    <row r="79" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79" s="42">
+        <f t="shared" si="5"/>
+        <v>48201.173600000329</v>
+      </c>
       <c r="D79" s="38">
         <v>2463621.5822000001</v>
       </c>
       <c r="E79" s="39"/>
       <c r="F79" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.838800000026822</v>
       </c>
       <c r="G79" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>83.664502229101544</v>
       </c>
       <c r="H79" s="38"/>
@@ -13643,17 +13956,21 @@
       <c r="L79" s="39"/>
       <c r="M79" s="39"/>
     </row>
-    <row r="80" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80" s="42">
+        <f t="shared" si="5"/>
+        <v>48284.968700000085</v>
+      </c>
       <c r="D80" s="38">
         <v>2463705.3772999998</v>
       </c>
       <c r="E80" s="39"/>
       <c r="F80" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.795099999755621</v>
       </c>
       <c r="G80" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>83.889314770653087</v>
       </c>
       <c r="H80" s="38"/>
@@ -13663,17 +13980,21 @@
       <c r="L80" s="39"/>
       <c r="M80" s="39"/>
     </row>
-    <row r="81" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81" s="42">
+        <f t="shared" si="5"/>
+        <v>48368.440900000278</v>
+      </c>
       <c r="D81" s="38">
         <v>2463788.8495</v>
       </c>
       <c r="E81" s="39"/>
       <c r="F81" s="40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.47220000019297</v>
       </c>
       <c r="G81" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>83.818803393389544</v>
       </c>
       <c r="H81" s="38"/>
@@ -13683,17 +14004,21 @@
       <c r="L81" s="39"/>
       <c r="M81" s="39"/>
     </row>
-    <row r="82" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82" s="42">
+        <f t="shared" si="5"/>
+        <v>48451.395200000145</v>
+      </c>
       <c r="D82" s="38">
         <v>2463871.8037999999</v>
       </c>
       <c r="E82" s="39"/>
       <c r="F82" s="40">
-        <f t="shared" ref="F82:F95" si="4">D82-D81</f>
+        <f t="shared" ref="F82:F95" si="6">D82-D81</f>
         <v>82.954299999866635</v>
       </c>
       <c r="G82" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>83.478091986562887</v>
       </c>
       <c r="H82" s="38"/>
@@ -13703,17 +14028,21 @@
       <c r="L82" s="39"/>
       <c r="M82" s="39"/>
     </row>
-    <row r="83" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A83" s="42">
+        <f t="shared" si="5"/>
+        <v>48533.829100000206</v>
+      </c>
       <c r="D83" s="38">
         <v>2463954.2376999999</v>
       </c>
       <c r="E83" s="39"/>
       <c r="F83" s="40">
+        <f t="shared" si="6"/>
+        <v>82.43390000006184</v>
+      </c>
+      <c r="G83" s="38">
         <f t="shared" si="4"/>
-        <v>82.43390000006184</v>
-      </c>
-      <c r="G83" s="38">
-        <f t="shared" si="3"/>
         <v>82.971120460026057</v>
       </c>
       <c r="H83" s="38"/>
@@ -13723,17 +14052,21 @@
       <c r="L83" s="39"/>
       <c r="M83" s="39"/>
     </row>
-    <row r="84" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A84" s="42">
+        <f t="shared" si="5"/>
+        <v>48615.927400000393</v>
+      </c>
       <c r="D84" s="38">
         <v>2464036.3360000001</v>
       </c>
       <c r="E84" s="39"/>
       <c r="F84" s="40">
+        <f t="shared" si="6"/>
+        <v>82.09830000018701</v>
+      </c>
+      <c r="G84" s="38">
         <f t="shared" si="4"/>
-        <v>82.09830000018701</v>
-      </c>
-      <c r="G84" s="38">
-        <f t="shared" si="3"/>
         <v>82.445502774902025</v>
       </c>
       <c r="H84" s="38"/>
@@ -13743,17 +14076,21 @@
       <c r="L84" s="39"/>
       <c r="M84" s="39"/>
     </row>
-    <row r="85" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A85" s="42">
+        <f t="shared" si="5"/>
+        <v>48697.951200000476</v>
+      </c>
       <c r="D85" s="38">
         <v>2464118.3598000002</v>
       </c>
       <c r="E85" s="39"/>
       <c r="F85" s="40">
+        <f t="shared" si="6"/>
+        <v>82.023800000082701</v>
+      </c>
+      <c r="G85" s="38">
         <f t="shared" si="4"/>
-        <v>82.023800000082701</v>
-      </c>
-      <c r="G85" s="38">
-        <f t="shared" si="3"/>
         <v>82.050887298841545</v>
       </c>
       <c r="H85" s="38"/>
@@ -13763,17 +14100,21 @@
       <c r="L85" s="39"/>
       <c r="M85" s="39"/>
     </row>
-    <row r="86" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A86" s="42">
+        <f t="shared" si="5"/>
+        <v>48780.165300000459</v>
+      </c>
       <c r="D86" s="38">
         <v>2464200.5739000002</v>
       </c>
       <c r="E86" s="39"/>
       <c r="F86" s="40">
+        <f t="shared" si="6"/>
+        <v>82.214099999982864</v>
+      </c>
+      <c r="G86" s="38">
         <f t="shared" si="4"/>
-        <v>82.214099999982864</v>
-      </c>
-      <c r="G86" s="38">
-        <f t="shared" si="3"/>
         <v>81.90008113987227</v>
       </c>
       <c r="H86" s="38"/>
@@ -13783,17 +14124,21 @@
       <c r="L86" s="39"/>
       <c r="M86" s="39"/>
     </row>
-    <row r="87" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A87" s="42">
+        <f t="shared" si="5"/>
+        <v>48862.779300000053</v>
+      </c>
       <c r="D87" s="38">
         <v>2464283.1878999998</v>
       </c>
       <c r="E87" s="39"/>
       <c r="F87" s="40">
+        <f t="shared" si="6"/>
+        <v>82.613999999593943</v>
+      </c>
+      <c r="G87" s="38">
         <f t="shared" si="4"/>
-        <v>82.613999999593943</v>
-      </c>
-      <c r="G87" s="38">
-        <f t="shared" si="3"/>
         <v>82.039048971142734</v>
       </c>
       <c r="H87" s="38"/>
@@ -13803,17 +14148,21 @@
       <c r="L87" s="39"/>
       <c r="M87" s="39"/>
     </row>
-    <row r="88" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A88" s="42">
+        <f t="shared" si="5"/>
+        <v>48945.873300000094</v>
+      </c>
       <c r="D88" s="38">
         <v>2464366.2818999998</v>
       </c>
       <c r="E88" s="39"/>
       <c r="F88" s="40">
+        <f t="shared" si="6"/>
+        <v>83.094000000040978</v>
+      </c>
+      <c r="G88" s="38">
         <f t="shared" si="4"/>
-        <v>83.094000000040978</v>
-      </c>
-      <c r="G88" s="38">
-        <f t="shared" si="3"/>
         <v>82.431526093885012</v>
       </c>
       <c r="H88" s="38"/>
@@ -13823,17 +14172,21 @@
       <c r="L88" s="39"/>
       <c r="M88" s="39"/>
     </row>
-    <row r="89" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A89" s="42">
+        <f t="shared" si="5"/>
+        <v>49029.376700000372</v>
+      </c>
       <c r="D89" s="38">
         <v>2464449.7853000001</v>
       </c>
       <c r="E89" s="39"/>
       <c r="F89" s="40">
+        <f t="shared" si="6"/>
+        <v>83.503400000277907</v>
+      </c>
+      <c r="G89" s="38">
         <f t="shared" si="4"/>
-        <v>83.503400000277907</v>
-      </c>
-      <c r="G89" s="38">
-        <f t="shared" si="3"/>
         <v>82.964673622939728</v>
       </c>
       <c r="H89" s="38"/>
@@ -13843,17 +14196,21 @@
       <c r="L89" s="39"/>
       <c r="M89" s="39"/>
     </row>
-    <row r="90" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A90" s="42">
+        <f t="shared" si="5"/>
+        <v>49113.118700000457</v>
+      </c>
       <c r="D90" s="38">
         <v>2464533.5273000002</v>
       </c>
       <c r="E90" s="39"/>
       <c r="F90" s="40">
+        <f t="shared" si="6"/>
+        <v>83.742000000085682</v>
+      </c>
+      <c r="G90" s="38">
         <f t="shared" si="4"/>
-        <v>83.742000000085682</v>
-      </c>
-      <c r="G90" s="38">
-        <f t="shared" si="3"/>
         <v>83.479877458865474</v>
       </c>
       <c r="H90" s="38"/>
@@ -13863,17 +14220,21 @@
       <c r="L90" s="39"/>
       <c r="M90" s="39"/>
     </row>
-    <row r="91" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A91" s="42">
+        <f t="shared" si="5"/>
+        <v>49196.858600000385</v>
+      </c>
       <c r="D91" s="38">
         <v>2464617.2672000001</v>
       </c>
       <c r="E91" s="39"/>
       <c r="F91" s="40">
+        <f t="shared" si="6"/>
+        <v>83.739899999927729</v>
+      </c>
+      <c r="G91" s="38">
         <f t="shared" si="4"/>
-        <v>83.739899999927729</v>
-      </c>
-      <c r="G91" s="38">
-        <f t="shared" si="3"/>
         <v>83.821693564913289</v>
       </c>
       <c r="H91" s="38"/>
@@ -13883,17 +14244,21 @@
       <c r="L91" s="39"/>
       <c r="M91" s="39"/>
     </row>
-    <row r="92" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A92" s="42">
+        <f t="shared" si="5"/>
+        <v>49280.322800000198</v>
+      </c>
       <c r="D92" s="38">
         <v>2464700.7313999999</v>
       </c>
       <c r="E92" s="39"/>
       <c r="F92" s="40">
+        <f t="shared" si="6"/>
+        <v>83.46419999981299</v>
+      </c>
+      <c r="G92" s="38">
         <f t="shared" si="4"/>
-        <v>83.46419999981299</v>
-      </c>
-      <c r="G92" s="38">
-        <f t="shared" si="3"/>
         <v>83.888219093276504</v>
       </c>
       <c r="H92" s="38"/>
@@ -13903,17 +14268,21 @@
       <c r="L92" s="39"/>
       <c r="M92" s="39"/>
     </row>
-    <row r="93" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A93" s="42">
+        <f t="shared" si="5"/>
+        <v>49363.300600000191</v>
+      </c>
       <c r="D93" s="38">
         <v>2464783.7091999999</v>
       </c>
       <c r="E93" s="39"/>
       <c r="F93" s="40">
+        <f t="shared" si="6"/>
+        <v>82.977799999993294</v>
+      </c>
+      <c r="G93" s="38">
         <f t="shared" si="4"/>
-        <v>82.977799999993294</v>
-      </c>
-      <c r="G93" s="38">
-        <f t="shared" si="3"/>
         <v>83.663258441856655</v>
       </c>
       <c r="H93" s="38"/>
@@ -13923,17 +14292,21 @@
       <c r="L93" s="39"/>
       <c r="M93" s="39"/>
     </row>
-    <row r="94" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A94" s="42">
+        <f t="shared" si="5"/>
+        <v>49445.764400000218</v>
+      </c>
       <c r="D94" s="38">
         <v>2464866.173</v>
       </c>
       <c r="E94" s="39"/>
       <c r="F94" s="40">
+        <f t="shared" si="6"/>
+        <v>82.463800000026822</v>
+      </c>
+      <c r="G94" s="38">
         <f t="shared" si="4"/>
-        <v>82.463800000026822</v>
-      </c>
-      <c r="G94" s="38">
-        <f t="shared" si="3"/>
         <v>83.217352045195341</v>
       </c>
       <c r="H94" s="38"/>
@@ -13943,17 +14316,21 @@
       <c r="L94" s="39"/>
       <c r="M94" s="39"/>
     </row>
-    <row r="95" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A95" s="42">
+        <f t="shared" si="5"/>
+        <v>49527.88170000026</v>
+      </c>
       <c r="D95" s="38">
         <v>2464948.2903</v>
       </c>
       <c r="E95" s="39"/>
       <c r="F95" s="40">
+        <f t="shared" si="6"/>
+        <v>82.117300000041723</v>
+      </c>
+      <c r="G95" s="38">
         <f t="shared" si="4"/>
-        <v>82.117300000041723</v>
-      </c>
-      <c r="G95" s="38">
-        <f t="shared" si="3"/>
         <v>82.681596646151021</v>
       </c>
       <c r="H95" s="38"/>
@@ -13963,7 +14340,11 @@
       <c r="L95" s="39"/>
       <c r="M95" s="39"/>
     </row>
-    <row r="96" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A96" s="42">
+        <f t="shared" si="5"/>
+        <v>42980.99799722014</v>
+      </c>
       <c r="D96" s="37">
         <v>2458401.4065972199</v>
       </c>
@@ -13977,7 +14358,11 @@
       <c r="L96" s="39"/>
       <c r="M96" s="39"/>
     </row>
-    <row r="97" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A97" s="42">
+        <f t="shared" si="5"/>
+        <v>43063.517094440293</v>
+      </c>
       <c r="D97" s="37">
         <v>2458483.92569444</v>
       </c>
@@ -13994,7 +14379,11 @@
       <c r="L97" s="39"/>
       <c r="M97" s="39"/>
     </row>
-    <row r="98" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A98" s="42">
+        <f t="shared" si="5"/>
+        <v>43146.486886110157</v>
+      </c>
       <c r="D98" s="37">
         <v>2458566.8954861099</v>
       </c>
@@ -14002,7 +14391,7 @@
       <c r="F98" s="40"/>
       <c r="G98" s="38"/>
       <c r="H98" s="38">
-        <f t="shared" ref="H98:H121" si="5">D98-D97</f>
+        <f t="shared" ref="H98:H121" si="7">D98-D97</f>
         <v>82.969791669864208</v>
       </c>
       <c r="I98" s="39"/>
@@ -14011,7 +14400,11 @@
       <c r="L98" s="39"/>
       <c r="M98" s="39"/>
     </row>
-    <row r="99" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A99" s="42">
+        <f t="shared" si="5"/>
+        <v>43229.991747220047</v>
+      </c>
       <c r="D99" s="37">
         <v>2458650.4003472198</v>
       </c>
@@ -14019,7 +14412,7 @@
       <c r="F99" s="40"/>
       <c r="G99" s="38"/>
       <c r="H99" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>83.504861109890044</v>
       </c>
       <c r="I99" s="39"/>
@@ -14028,7 +14421,11 @@
       <c r="L99" s="39"/>
       <c r="M99" s="39"/>
     </row>
-    <row r="100" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A100" s="42">
+        <f t="shared" si="5"/>
+        <v>43313.878552770242</v>
+      </c>
       <c r="D100" s="37">
         <v>2458734.28715277</v>
       </c>
@@ -14036,7 +14433,7 @@
       <c r="F100" s="40"/>
       <c r="G100" s="38"/>
       <c r="H100" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>83.886805550195277</v>
       </c>
       <c r="I100" s="39"/>
@@ -14045,7 +14442,11 @@
       <c r="L100" s="39"/>
       <c r="M100" s="39"/>
     </row>
-    <row r="101" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A101" s="42">
+        <f t="shared" si="5"/>
+        <v>43397.889663880225</v>
+      </c>
       <c r="D101" s="37">
         <v>2458818.29826388</v>
       </c>
@@ -14053,7 +14454,7 @@
       <c r="F101" s="40"/>
       <c r="G101" s="38"/>
       <c r="H101" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>84.011111109983176</v>
       </c>
       <c r="I101" s="39"/>
@@ -14062,7 +14463,11 @@
       <c r="L101" s="39"/>
       <c r="M101" s="39"/>
     </row>
-    <row r="102" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A102" s="42">
+        <f t="shared" si="5"/>
+        <v>43481.808413880412</v>
+      </c>
       <c r="D102" s="37">
         <v>2458902.2170138801</v>
       </c>
@@ -14070,7 +14475,7 @@
       <c r="F102" s="40"/>
       <c r="G102" s="38"/>
       <c r="H102" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>83.918750000186265</v>
       </c>
       <c r="I102" s="39"/>
@@ -14079,7 +14484,11 @@
       <c r="L102" s="39"/>
       <c r="M102" s="39"/>
     </row>
-    <row r="103" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A103" s="42">
+        <f t="shared" si="5"/>
+        <v>43565.480636110064</v>
+      </c>
       <c r="D103" s="37">
         <v>2458985.8892361098</v>
       </c>
@@ -14087,7 +14496,7 @@
       <c r="F103" s="40"/>
       <c r="G103" s="38"/>
       <c r="H103" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>83.672222229652107</v>
       </c>
       <c r="I103" s="39"/>
@@ -14096,7 +14505,11 @@
       <c r="L103" s="39"/>
       <c r="M103" s="39"/>
     </row>
-    <row r="104" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A104" s="42">
+        <f t="shared" si="5"/>
+        <v>43648.813622220419</v>
+      </c>
       <c r="D104" s="37">
         <v>2459069.2222222202</v>
       </c>
@@ -14104,7 +14517,7 @@
       <c r="F104" s="40"/>
       <c r="G104" s="38"/>
       <c r="H104" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>83.332986110355705</v>
       </c>
       <c r="I104" s="39"/>
@@ -14113,7 +14526,11 @@
       <c r="L104" s="39"/>
       <c r="M104" s="39"/>
     </row>
-    <row r="105" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A105" s="42">
+        <f t="shared" si="5"/>
+        <v>43731.791747220326</v>
+      </c>
       <c r="D105" s="37">
         <v>2459152.2003472201</v>
       </c>
@@ -14121,7 +14538,7 @@
       <c r="F105" s="40"/>
       <c r="G105" s="38"/>
       <c r="H105" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>82.978124999906868</v>
       </c>
       <c r="I105" s="39"/>
@@ -14130,7 +14547,11 @@
       <c r="L105" s="39"/>
       <c r="M105" s="39"/>
     </row>
-    <row r="106" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A106" s="42">
+        <f t="shared" si="5"/>
+        <v>43814.471955550369</v>
+      </c>
       <c r="D106" s="37">
         <v>2459234.8805555501</v>
       </c>
@@ -14138,7 +14559,7 @@
       <c r="F106" s="40"/>
       <c r="G106" s="38"/>
       <c r="H106" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>82.68020833004266</v>
       </c>
       <c r="I106" s="39"/>
@@ -14147,7 +14568,11 @@
       <c r="L106" s="39"/>
       <c r="M106" s="39"/>
     </row>
-    <row r="107" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A107" s="42">
+        <f t="shared" si="5"/>
+        <v>43896.953552770428</v>
+      </c>
       <c r="D107" s="37">
         <v>2459317.3621527702</v>
       </c>
@@ -14155,7 +14580,7 @@
       <c r="F107" s="40"/>
       <c r="G107" s="38"/>
       <c r="H107" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>82.481597220059484</v>
       </c>
       <c r="I107" s="39"/>
@@ -14164,7 +14589,11 @@
       <c r="L107" s="39"/>
       <c r="M107" s="39"/>
     </row>
-    <row r="108" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A108" s="42">
+        <f t="shared" si="5"/>
+        <v>43979.346955550369</v>
+      </c>
       <c r="D108" s="37">
         <v>2459399.7555555501</v>
       </c>
@@ -14172,7 +14601,7 @@
       <c r="F108" s="40"/>
       <c r="G108" s="38"/>
       <c r="H108" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>82.393402779940516</v>
       </c>
       <c r="I108" s="39"/>
@@ -14181,7 +14610,11 @@
       <c r="L108" s="39"/>
       <c r="M108" s="39"/>
     </row>
-    <row r="109" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A109" s="42">
+        <f t="shared" si="5"/>
+        <v>44061.759455550462</v>
+      </c>
       <c r="D109" s="37">
         <v>2459482.1680555502</v>
       </c>
@@ -14189,7 +14622,7 @@
       <c r="F109" s="40"/>
       <c r="G109" s="38"/>
       <c r="H109" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>82.412500000093132</v>
       </c>
       <c r="I109" s="39"/>
@@ -14198,7 +14631,11 @@
       <c r="L109" s="39"/>
       <c r="M109" s="39"/>
     </row>
-    <row r="110" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A110" s="42">
+        <f t="shared" si="5"/>
+        <v>44144.296608330216</v>
+      </c>
       <c r="D110" s="37">
         <v>2459564.7052083299</v>
       </c>
@@ -14206,7 +14643,7 @@
       <c r="F110" s="40"/>
       <c r="G110" s="38"/>
       <c r="H110" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>82.537152779754251</v>
       </c>
       <c r="I110" s="39"/>
@@ -14215,7 +14652,11 @@
       <c r="L110" s="39"/>
       <c r="M110" s="39"/>
     </row>
-    <row r="111" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A111" s="42">
+        <f t="shared" si="5"/>
+        <v>44227.064316660166</v>
+      </c>
       <c r="D111" s="37">
         <v>2459647.4729166599</v>
       </c>
@@ -14223,7 +14664,7 @@
       <c r="F111" s="40"/>
       <c r="G111" s="38"/>
       <c r="H111" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>82.767708329949528</v>
       </c>
       <c r="I111" s="39"/>
@@ -14232,7 +14673,11 @@
       <c r="L111" s="39"/>
       <c r="M111" s="39"/>
     </row>
-    <row r="112" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A112" s="42">
+        <f t="shared" si="5"/>
+        <v>44310.154941660352</v>
+      </c>
       <c r="D112" s="37">
         <v>2459730.5635416601</v>
       </c>
@@ -14240,7 +14685,7 @@
       <c r="F112" s="40"/>
       <c r="G112" s="38"/>
       <c r="H112" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>83.090625000186265</v>
       </c>
       <c r="I112" s="39"/>
@@ -14249,7 +14694,11 @@
       <c r="L112" s="39"/>
       <c r="M112" s="39"/>
     </row>
-    <row r="113" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A113" s="42">
+        <f t="shared" si="5"/>
+        <v>44393.616747220047</v>
+      </c>
       <c r="D113" s="37">
         <v>2459814.0253472198</v>
       </c>
@@ -14257,7 +14706,7 @@
       <c r="F113" s="40"/>
       <c r="G113" s="38"/>
       <c r="H113" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>83.461805559694767</v>
       </c>
       <c r="I113" s="39"/>
@@ -14266,7 +14715,11 @@
       <c r="L113" s="39"/>
       <c r="M113" s="39"/>
     </row>
-    <row r="114" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A114" s="42">
+        <f t="shared" si="5"/>
+        <v>44477.407372220419</v>
+      </c>
       <c r="D114" s="37">
         <v>2459897.8159722202</v>
       </c>
@@ -14274,7 +14727,7 @@
       <c r="F114" s="40"/>
       <c r="G114" s="38"/>
       <c r="H114" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>83.790625000372529</v>
       </c>
       <c r="I114" s="39"/>
@@ -14283,7 +14736,11 @@
       <c r="L114" s="39"/>
       <c r="M114" s="39"/>
     </row>
-    <row r="115" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A115" s="42">
+        <f t="shared" si="5"/>
+        <v>44561.377163880039</v>
+      </c>
       <c r="D115" s="37">
         <v>2459981.7857638798</v>
       </c>
@@ -14291,7 +14748,7 @@
       <c r="F115" s="40"/>
       <c r="G115" s="38"/>
       <c r="H115" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>83.969791659619659</v>
       </c>
       <c r="I115" s="39"/>
@@ -14300,7 +14757,11 @@
       <c r="L115" s="39"/>
       <c r="M115" s="39"/>
     </row>
-    <row r="116" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A116" s="42">
+        <f t="shared" si="5"/>
+        <v>44645.302163880318</v>
+      </c>
       <c r="D116" s="37">
         <v>2460065.7107638801</v>
       </c>
@@ -14308,7 +14769,7 @@
       <c r="F116" s="40"/>
       <c r="G116" s="38"/>
       <c r="H116" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>83.925000000279397</v>
       </c>
       <c r="I116" s="39"/>
@@ -14317,7 +14778,11 @@
       <c r="L116" s="39"/>
       <c r="M116" s="39"/>
     </row>
-    <row r="117" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A117" s="42">
+        <f t="shared" si="5"/>
+        <v>44728.961538880132</v>
+      </c>
       <c r="D117" s="37">
         <v>2460149.3701388799</v>
       </c>
@@ -14325,7 +14790,7 @@
       <c r="F117" s="40"/>
       <c r="G117" s="38"/>
       <c r="H117" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>83.659374999813735</v>
       </c>
       <c r="I117" s="39"/>
@@ -14334,7 +14799,11 @@
       <c r="L117" s="39"/>
       <c r="M117" s="39"/>
     </row>
-    <row r="118" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A118" s="42">
+        <f t="shared" si="5"/>
+        <v>44812.215011110064</v>
+      </c>
       <c r="D118" s="37">
         <v>2460232.6236111098</v>
       </c>
@@ -14342,7 +14811,7 @@
       <c r="F118" s="40"/>
       <c r="G118" s="38"/>
       <c r="H118" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>83.253472229931504</v>
       </c>
       <c r="I118" s="39"/>
@@ -14351,7 +14820,11 @@
       <c r="L118" s="39"/>
       <c r="M118" s="39"/>
     </row>
-    <row r="119" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A119" s="42">
+        <f t="shared" si="5"/>
+        <v>44895.084455550183</v>
+      </c>
       <c r="D119" s="37">
         <v>2460315.4930555499</v>
       </c>
@@ -14359,7 +14832,7 @@
       <c r="F119" s="40"/>
       <c r="G119" s="38"/>
       <c r="H119" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>82.869444440118968</v>
       </c>
       <c r="I119" s="39"/>
@@ -14368,7 +14841,11 @@
       <c r="L119" s="39"/>
       <c r="M119" s="39"/>
     </row>
-    <row r="120" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A120" s="42">
+        <f t="shared" si="5"/>
+        <v>44977.707719440106</v>
+      </c>
       <c r="D120" s="37">
         <v>2460398.1163194398</v>
       </c>
@@ -14376,7 +14853,7 @@
       <c r="F120" s="40"/>
       <c r="G120" s="38"/>
       <c r="H120" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>82.623263889923692</v>
       </c>
       <c r="I120" s="39"/>
@@ -14385,7 +14862,11 @@
       <c r="L120" s="39"/>
       <c r="M120" s="39"/>
     </row>
-    <row r="121" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A121" s="42">
+        <f t="shared" si="5"/>
+        <v>45060.261191660073</v>
+      </c>
       <c r="D121" s="37">
         <v>2460480.6697916598</v>
       </c>
@@ -14393,7 +14874,7 @@
       <c r="F121" s="40"/>
       <c r="G121" s="38"/>
       <c r="H121" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>82.553472219966352</v>
       </c>
       <c r="I121" s="39"/>
@@ -14402,7 +14883,8 @@
       <c r="L121" s="39"/>
       <c r="M121" s="39"/>
     </row>
-    <row r="122" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A122" s="42"/>
       <c r="D122" s="39"/>
       <c r="E122" s="39"/>
       <c r="F122" s="39"/>
@@ -14414,7 +14896,7 @@
       <c r="L122" s="39"/>
       <c r="M122" s="39"/>
     </row>
-    <row r="123" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D123" s="39"/>
       <c r="E123" s="39"/>
       <c r="F123" s="39"/>
@@ -14426,7 +14908,7 @@
       <c r="L123" s="39"/>
       <c r="M123" s="39"/>
     </row>
-    <row r="124" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D124" s="39"/>
       <c r="E124" s="39"/>
       <c r="F124" s="39"/>
@@ -14438,7 +14920,7 @@
       <c r="L124" s="39"/>
       <c r="M124" s="39"/>
     </row>
-    <row r="125" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D125" s="39"/>
       <c r="E125" s="39"/>
       <c r="F125" s="39"/>
@@ -14450,7 +14932,7 @@
       <c r="L125" s="39"/>
       <c r="M125" s="39"/>
     </row>
-    <row r="126" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D126" s="39"/>
       <c r="E126" s="39"/>
       <c r="F126" s="39"/>
@@ -14462,7 +14944,7 @@
       <c r="L126" s="39"/>
       <c r="M126" s="39"/>
     </row>
-    <row r="127" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D127" s="39"/>
       <c r="E127" s="39"/>
       <c r="F127" s="39"/>
@@ -14474,7 +14956,7 @@
       <c r="L127" s="39"/>
       <c r="M127" s="39"/>
     </row>
-    <row r="128" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D128" s="39"/>
       <c r="E128" s="39"/>
       <c r="F128" s="39"/>

</xml_diff>